<commit_message>
Add conti-ord and contin-nom tests, and fix bug
</commit_message>
<xml_diff>
--- a/data/dataset_clean.xlsx
+++ b/data/dataset_clean.xlsx
@@ -681,16 +681,16 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G2">
         <v>2</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -699,10 +699,10 @@
         <v>2</v>
       </c>
       <c r="L2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N2">
         <v>2</v>
@@ -866,16 +866,16 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
         <v>2</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -884,10 +884,10 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N3">
         <v>2</v>
@@ -1051,16 +1051,16 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4">
         <v>2</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1069,10 +1069,10 @@
         <v>2</v>
       </c>
       <c r="L4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>2</v>
@@ -1236,16 +1236,16 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -1254,10 +1254,10 @@
         <v>2</v>
       </c>
       <c r="L5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5">
         <v>2</v>
@@ -1439,10 +1439,10 @@
         <v>2</v>
       </c>
       <c r="L6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>2</v>
@@ -1624,10 +1624,10 @@
         <v>2</v>
       </c>
       <c r="L7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7">
         <v>2</v>
@@ -2179,10 +2179,10 @@
         <v>2</v>
       </c>
       <c r="L10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10">
         <v>2</v>
@@ -2361,13 +2361,13 @@
         <v>2</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L11">
         <v>2</v>
       </c>
       <c r="M11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N11">
         <v>2</v>
@@ -2716,13 +2716,13 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <v>2</v>
       </c>
       <c r="H13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2734,10 +2734,10 @@
         <v>2</v>
       </c>
       <c r="L13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N13">
         <v>2</v>
@@ -2901,16 +2901,16 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>2</v>
       </c>
       <c r="H14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14">
         <v>2</v>
@@ -2919,10 +2919,10 @@
         <v>2</v>
       </c>
       <c r="L14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N14">
         <v>2</v>
@@ -3086,16 +3086,16 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>2</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15">
         <v>2</v>
@@ -3104,10 +3104,10 @@
         <v>2</v>
       </c>
       <c r="L15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <v>2</v>
@@ -3288,13 +3288,13 @@
         <v>1</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17">
         <v>2</v>
       </c>
       <c r="H17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I17">
         <v>2</v>
@@ -3306,10 +3306,10 @@
         <v>2</v>
       </c>
       <c r="L17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M17">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N17">
         <v>2</v>
@@ -3491,10 +3491,10 @@
         <v>2</v>
       </c>
       <c r="L18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M18">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N18">
         <v>2</v>
@@ -3675,13 +3675,13 @@
         <v>1</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20">
         <v>2</v>
@@ -3860,13 +3860,13 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I21">
         <v>2</v>
@@ -4045,13 +4045,13 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G22">
         <v>2</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I22">
         <v>2</v>
@@ -4230,13 +4230,13 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G23">
         <v>2</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23">
         <v>2</v>
@@ -4248,10 +4248,10 @@
         <v>2</v>
       </c>
       <c r="L23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N23">
         <v>2</v>
@@ -4415,13 +4415,13 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>2</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24">
         <v>2</v>
@@ -4433,10 +4433,10 @@
         <v>2</v>
       </c>
       <c r="L24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N24">
         <v>2</v>
@@ -4600,16 +4600,16 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G25">
         <v>2</v>
       </c>
       <c r="H25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -4618,10 +4618,10 @@
         <v>2</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N25">
         <v>2</v>
@@ -4785,13 +4785,13 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G26">
         <v>2</v>
       </c>
       <c r="H26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I26">
         <v>2</v>
@@ -4970,16 +4970,16 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G27">
         <v>2</v>
       </c>
       <c r="H27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27">
         <v>2</v>
@@ -4988,10 +4988,10 @@
         <v>2</v>
       </c>
       <c r="L27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N27">
         <v>2</v>
@@ -5155,16 +5155,16 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G28">
         <v>2</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28">
         <v>2</v>
@@ -5173,10 +5173,10 @@
         <v>2</v>
       </c>
       <c r="L28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M28">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N28">
         <v>2</v>
@@ -5340,16 +5340,16 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>2</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29">
         <v>2</v>
@@ -5358,13 +5358,13 @@
         <v>2</v>
       </c>
       <c r="L29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N29">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O29">
         <v>1</v>
@@ -5525,16 +5525,16 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G30">
         <v>2</v>
       </c>
       <c r="H30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30">
         <v>2</v>
@@ -5710,16 +5710,16 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G31">
         <v>2</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31">
         <v>2</v>
@@ -5728,10 +5728,10 @@
         <v>2</v>
       </c>
       <c r="L31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N31">
         <v>2</v>
@@ -5895,16 +5895,16 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G32">
         <v>2</v>
       </c>
       <c r="H32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32">
         <v>2</v>
@@ -5913,10 +5913,10 @@
         <v>2</v>
       </c>
       <c r="L32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N32">
         <v>2</v>
@@ -6097,13 +6097,13 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G34">
         <v>2</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <v>2</v>
@@ -6282,13 +6282,13 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G35">
         <v>2</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>2</v>
@@ -6300,10 +6300,10 @@
         <v>2</v>
       </c>
       <c r="L35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N35">
         <v>2</v>
@@ -6467,16 +6467,16 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G36">
         <v>2</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36">
         <v>2</v>
@@ -6485,10 +6485,10 @@
         <v>2</v>
       </c>
       <c r="L36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N36">
         <v>2</v>
@@ -6652,13 +6652,13 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G37">
         <v>2</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I37">
         <v>2</v>
@@ -6670,10 +6670,10 @@
         <v>2</v>
       </c>
       <c r="L37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M37">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N37">
         <v>2</v>
@@ -6855,10 +6855,10 @@
         <v>2</v>
       </c>
       <c r="L38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M38">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N38">
         <v>2</v>
@@ -7022,16 +7022,16 @@
         <v>1</v>
       </c>
       <c r="F39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G39">
         <v>2</v>
       </c>
       <c r="H39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I39">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39">
         <v>2</v>
@@ -7225,13 +7225,13 @@
         <v>2</v>
       </c>
       <c r="L40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O40">
         <v>1</v>
@@ -7392,13 +7392,13 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G41">
         <v>2</v>
       </c>
       <c r="H41">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I41">
         <v>2</v>
@@ -7577,16 +7577,16 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G42">
         <v>2</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J42">
         <v>2</v>
@@ -7762,13 +7762,13 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G43">
         <v>2</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I43">
         <v>2</v>
@@ -7777,10 +7777,10 @@
         <v>2</v>
       </c>
       <c r="K43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L43">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M43">
         <v>2</v>
@@ -8149,13 +8149,13 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G46">
         <v>2</v>
       </c>
       <c r="H46">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I46">
         <v>2</v>
@@ -8519,13 +8519,13 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G48">
         <v>2</v>
       </c>
       <c r="H48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I48">
         <v>2</v>
@@ -8537,10 +8537,10 @@
         <v>2</v>
       </c>
       <c r="L48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M48">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N48">
         <v>2</v>
@@ -8704,16 +8704,16 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G49">
         <v>2</v>
       </c>
       <c r="H49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49">
         <v>2</v>
@@ -9074,13 +9074,13 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G51">
         <v>2</v>
       </c>
       <c r="H51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I51">
         <v>2</v>
@@ -9092,10 +9092,10 @@
         <v>2</v>
       </c>
       <c r="L51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N51">
         <v>2</v>
@@ -9259,16 +9259,16 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G52">
         <v>2</v>
       </c>
       <c r="H52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52">
         <v>2</v>
@@ -9277,13 +9277,13 @@
         <v>2</v>
       </c>
       <c r="L52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N52">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O52">
         <v>1</v>
@@ -9444,7 +9444,7 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G53">
         <v>2</v>
@@ -9453,7 +9453,7 @@
         <v>2</v>
       </c>
       <c r="I53">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J53">
         <v>2</v>
@@ -9629,13 +9629,13 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G54">
         <v>2</v>
       </c>
       <c r="H54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I54">
         <v>2</v>
@@ -9647,10 +9647,10 @@
         <v>2</v>
       </c>
       <c r="L54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N54">
         <v>2</v>
@@ -9832,10 +9832,10 @@
         <v>2</v>
       </c>
       <c r="L55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M55">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N55">
         <v>2</v>
@@ -9999,13 +9999,13 @@
         <v>1</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G56">
         <v>2</v>
       </c>
       <c r="H56">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I56">
         <v>2</v>
@@ -10404,10 +10404,10 @@
         <v>2</v>
       </c>
       <c r="L59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M59">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N59">
         <v>2</v>
@@ -10807,16 +10807,16 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G64">
         <v>2</v>
       </c>
       <c r="H64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J64">
         <v>2</v>
@@ -10825,10 +10825,10 @@
         <v>2</v>
       </c>
       <c r="L64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M64">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N64">
         <v>2</v>
@@ -11010,10 +11010,10 @@
         <v>2</v>
       </c>
       <c r="L65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N65">
         <v>2</v>
@@ -11211,16 +11211,16 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G68">
         <v>2</v>
       </c>
       <c r="H68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J68">
         <v>2</v>
@@ -11229,10 +11229,10 @@
         <v>2</v>
       </c>
       <c r="L68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M68">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N68">
         <v>2</v>
@@ -11396,16 +11396,16 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G69">
         <v>2</v>
       </c>
       <c r="H69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I69">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J69">
         <v>2</v>
@@ -12338,13 +12338,13 @@
         <v>1</v>
       </c>
       <c r="F75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G75">
         <v>2</v>
       </c>
       <c r="H75">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I75">
         <v>2</v>
@@ -12523,16 +12523,16 @@
         <v>1</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J76">
         <v>2</v>
@@ -12726,10 +12726,10 @@
         <v>2</v>
       </c>
       <c r="L77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M77">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N77">
         <v>2</v>
@@ -12911,10 +12911,10 @@
         <v>2</v>
       </c>
       <c r="L78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M78">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N78">
         <v>2</v>

</xml_diff>